<commit_message>
new nra fig, updated code to 1ha, added metadata to NRA sheet, moved old code (incl NMDS trial) to extras
</commit_message>
<xml_diff>
--- a/nra_data.xlsx
+++ b/nra_data.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\2019\ANDAMAN from DESKTOP\Andamans\Andamans 2018\working\NRA_deciduousness\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Indian-Forester\andaman-logging-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7593C95A-E9DE-4902-BD58-065C9145DEC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299427A4-D8C2-42E1-BB7A-568A139006E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="metadata" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="metadata_sites" sheetId="2" r:id="rId2"/>
+    <sheet name="metadata_species" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">data!$A$1:$J$663</definedName>
@@ -898,15 +898,15 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="8.5703125" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="8.5703125" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -22137,7 +22137,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>